<commit_message>
fix normalize in fit2c
</commit_message>
<xml_diff>
--- a/logs/2c/2cresult.xlsx
+++ b/logs/2c/2cresult.xlsx
@@ -447,58 +447,58 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.2207931065074774</v>
+        <v>0.1290141311112389</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4495143367121741</v>
+        <v>0.2163186755499787</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.01447629266813791</v>
+        <v>0.008458807205688557</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3470388193189533</v>
+        <v>0.1670046350658946</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.001249136095300818</v>
+        <v>0.00072989691808817</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.2315371035762366</v>
+        <v>-0.1114220292785898</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.0816593526625094</v>
+        <v>0.04771530505415983</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2814659311757815</v>
+        <v>0.1354491558372081</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.2039051050119493</v>
+        <v>-0.1191461108926047</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.09417844302866619</v>
+        <v>-0.04532125985197404</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>0.584321372854409</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0.4812275335469187</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.3932091097986641</v>
+        <v>0.2297604868564154</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.07536729681338426</v>
+        <v>-0.03626881835560345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>